<commit_message>
Finalização Export Produtos Excel
</commit_message>
<xml_diff>
--- a/Pet_Shop/wwwroot/Temp/Produtos.xlsx
+++ b/Pet_Shop/wwwroot/Temp/Produtos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Imagem</t>
   </si>
@@ -38,16 +38,40 @@
     <t>Categoria</t>
   </si>
   <si>
-    <t>Teste</t>
+    <t>Boneco</t>
+  </si>
+  <si>
+    <t>Brinquedo de Borracha</t>
+  </si>
+  <si>
+    <t>Brinquedos</t>
+  </si>
+  <si>
+    <t>Areia</t>
+  </si>
+  <si>
+    <t>Areia Pipicat 2Kg</t>
+  </si>
+  <si>
+    <t>Limpeza</t>
+  </si>
+  <si>
+    <t>Pente</t>
+  </si>
+  <si>
+    <t>Tow Pente Fino</t>
+  </si>
+  <si>
+    <t>Ração</t>
+  </si>
+  <si>
+    <t>Wikas 2kg</t>
   </si>
   <si>
     <t>Alimento</t>
   </si>
   <si>
     <t>Ração Gato</t>
-  </si>
-  <si>
-    <t>Wikas 2kg</t>
   </si>
   <si>
     <t>Outros</t>
@@ -89,10 +113,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -102,106 +132,345 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>-1143000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>-1143000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1047750" cy="1047750"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" descr="" name="Boneco"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>-1143000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>-1143000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1047750" cy="1047750"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" descr="" name="Areia"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>-1143000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>-1143000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1047750" cy="1047750"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" descr="" name="Pente"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>-1143000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>-1143000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1047750" cy="1047750"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" descr="" name="Ração"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>-1143000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>-1143000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1047750" cy="1047750"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" descr="" name="Ração Gato"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="">
     <tabColor rgb="FF000000"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.849358558654785" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="10.7305908203125" customWidth="1"/>
-    <col min="4" max="4" width="9.550995826721191" customWidth="1"/>
+    <col min="4" max="4" width="20.97658920288086" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="11.30555248260498" customWidth="1"/>
     <col min="7" max="7" width="15.4315767288208" customWidth="1"/>
-    <col min="8" max="8" width="9.286023139953613" customWidth="1"/>
+    <col min="8" max="8" width="10.7091064453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>255</v>
-      </c>
-      <c r="B2" s="0">
+    <row r="2" ht="100" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" ht="100" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0">
-        <v>1</v>
-      </c>
-      <c r="F2" s="0">
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="G2" s="0">
-        <v>1</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0">
-        <v>255</v>
-      </c>
-      <c r="B3" s="0">
+      <c r="G3" s="3">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" ht="100" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0">
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" ht="100" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3">
+        <v>40</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" ht="100" customHeight="1">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3">
         <v>80</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F6" s="3">
         <v>30</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G6" s="3">
         <v>5</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>12</v>
+      <c r="H6" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reorganizei o Layout do Menu, remove Orçamento
</commit_message>
<xml_diff>
--- a/Pet_Shop/wwwroot/Temp/Produtos.xlsx
+++ b/Pet_Shop/wwwroot/Temp/Produtos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Imagem</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Ração Gato</t>
-  </si>
-  <si>
-    <t>Outros</t>
   </si>
 </sst>
 </file>
@@ -466,7 +463,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>